<commit_message>
Add 2018 yardage data and 2021 conference data. Also include logic to cut out current year before games are entered
</commit_message>
<xml_diff>
--- a/Data Files/Results.xlsx
+++ b/Data Files/Results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rspoonmore/Documents/Coding/CollegeFootballBowlGames/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rspoonmore/Documents/Coding/CollegeFootballBowlGames/Data Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A0A285-54B8-CF46-AEB6-7A73B90AF063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FAFC728-D9FE-CD45-B370-C838846059D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="250">
   <si>
     <t>School</t>
   </si>
@@ -1621,10 +1621,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M215"/>
+  <dimension ref="A1:M213"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A203" sqref="A203"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="F172" sqref="F172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7189,6 +7191,24 @@
       <c r="G136">
         <v>52</v>
       </c>
+      <c r="H136">
+        <v>313</v>
+      </c>
+      <c r="I136">
+        <v>556</v>
+      </c>
+      <c r="J136">
+        <v>120</v>
+      </c>
+      <c r="K136">
+        <v>197</v>
+      </c>
+      <c r="L136">
+        <v>193</v>
+      </c>
+      <c r="M136">
+        <v>359</v>
+      </c>
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
@@ -7212,6 +7232,30 @@
       <c r="G137">
         <v>13</v>
       </c>
+      <c r="H137">
+        <f>I136</f>
+        <v>556</v>
+      </c>
+      <c r="I137">
+        <f>H136</f>
+        <v>313</v>
+      </c>
+      <c r="J137">
+        <f>K136</f>
+        <v>197</v>
+      </c>
+      <c r="K137">
+        <f>J136</f>
+        <v>120</v>
+      </c>
+      <c r="L137">
+        <f>M136</f>
+        <v>359</v>
+      </c>
+      <c r="M137">
+        <f>L136</f>
+        <v>193</v>
+      </c>
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
@@ -7235,6 +7279,24 @@
       <c r="G138">
         <v>24</v>
       </c>
+      <c r="H138">
+        <v>482</v>
+      </c>
+      <c r="I138">
+        <v>258</v>
+      </c>
+      <c r="J138">
+        <v>337</v>
+      </c>
+      <c r="K138">
+        <v>84</v>
+      </c>
+      <c r="L138">
+        <v>145</v>
+      </c>
+      <c r="M138">
+        <v>174</v>
+      </c>
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
@@ -7258,6 +7320,30 @@
       <c r="G139">
         <v>41</v>
       </c>
+      <c r="H139">
+        <f>I138</f>
+        <v>258</v>
+      </c>
+      <c r="I139">
+        <f>H138</f>
+        <v>482</v>
+      </c>
+      <c r="J139">
+        <f>K138</f>
+        <v>84</v>
+      </c>
+      <c r="K139">
+        <f>J138</f>
+        <v>337</v>
+      </c>
+      <c r="L139">
+        <f>M138</f>
+        <v>174</v>
+      </c>
+      <c r="M139">
+        <f>L138</f>
+        <v>145</v>
+      </c>
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
@@ -7281,6 +7367,24 @@
       <c r="G140">
         <v>31</v>
       </c>
+      <c r="H140">
+        <v>293</v>
+      </c>
+      <c r="I140">
+        <v>436</v>
+      </c>
+      <c r="J140">
+        <v>164</v>
+      </c>
+      <c r="K140">
+        <v>260</v>
+      </c>
+      <c r="L140">
+        <v>129</v>
+      </c>
+      <c r="M140">
+        <v>176</v>
+      </c>
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
@@ -7304,6 +7408,30 @@
       <c r="G141">
         <v>20</v>
       </c>
+      <c r="H141">
+        <f t="shared" ref="H141" si="0">I140</f>
+        <v>436</v>
+      </c>
+      <c r="I141">
+        <f t="shared" ref="I141" si="1">H140</f>
+        <v>293</v>
+      </c>
+      <c r="J141">
+        <f t="shared" ref="J141" si="2">K140</f>
+        <v>260</v>
+      </c>
+      <c r="K141">
+        <f t="shared" ref="K141" si="3">J140</f>
+        <v>164</v>
+      </c>
+      <c r="L141">
+        <f t="shared" ref="L141" si="4">M140</f>
+        <v>176</v>
+      </c>
+      <c r="M141">
+        <f t="shared" ref="M141" si="5">L140</f>
+        <v>129</v>
+      </c>
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
@@ -7327,6 +7455,24 @@
       <c r="G142">
         <v>23</v>
       </c>
+      <c r="H142">
+        <v>301</v>
+      </c>
+      <c r="I142">
+        <v>364</v>
+      </c>
+      <c r="J142">
+        <v>97</v>
+      </c>
+      <c r="K142">
+        <v>331</v>
+      </c>
+      <c r="L142">
+        <v>204</v>
+      </c>
+      <c r="M142">
+        <v>33</v>
+      </c>
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
@@ -7350,6 +7496,30 @@
       <c r="G143">
         <v>21</v>
       </c>
+      <c r="H143">
+        <f t="shared" ref="H143" si="6">I142</f>
+        <v>364</v>
+      </c>
+      <c r="I143">
+        <f t="shared" ref="I143" si="7">H142</f>
+        <v>301</v>
+      </c>
+      <c r="J143">
+        <f t="shared" ref="J143" si="8">K142</f>
+        <v>331</v>
+      </c>
+      <c r="K143">
+        <f t="shared" ref="K143" si="9">J142</f>
+        <v>97</v>
+      </c>
+      <c r="L143">
+        <f t="shared" ref="L143" si="10">M142</f>
+        <v>33</v>
+      </c>
+      <c r="M143">
+        <f t="shared" ref="M143" si="11">L142</f>
+        <v>204</v>
+      </c>
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
@@ -7373,8 +7543,26 @@
       <c r="G144">
         <v>13</v>
       </c>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H144">
+        <v>448</v>
+      </c>
+      <c r="I144">
+        <v>392</v>
+      </c>
+      <c r="J144">
+        <v>233</v>
+      </c>
+      <c r="K144">
+        <v>62</v>
+      </c>
+      <c r="L144">
+        <v>215</v>
+      </c>
+      <c r="M144">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="145" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>244</v>
       </c>
@@ -7396,8 +7584,32 @@
       <c r="G145">
         <v>45</v>
       </c>
-    </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H145">
+        <f t="shared" ref="H145" si="12">I144</f>
+        <v>392</v>
+      </c>
+      <c r="I145">
+        <f t="shared" ref="I145" si="13">H144</f>
+        <v>448</v>
+      </c>
+      <c r="J145">
+        <f t="shared" ref="J145" si="14">K144</f>
+        <v>62</v>
+      </c>
+      <c r="K145">
+        <f t="shared" ref="K145" si="15">J144</f>
+        <v>233</v>
+      </c>
+      <c r="L145">
+        <f t="shared" ref="L145" si="16">M144</f>
+        <v>330</v>
+      </c>
+      <c r="M145">
+        <f t="shared" ref="M145" si="17">L144</f>
+        <v>215</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>122</v>
       </c>
@@ -7419,8 +7631,26 @@
       <c r="G146">
         <v>13</v>
       </c>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H146">
+        <v>476</v>
+      </c>
+      <c r="I146">
+        <v>287</v>
+      </c>
+      <c r="J146">
+        <v>103</v>
+      </c>
+      <c r="K146">
+        <v>108</v>
+      </c>
+      <c r="L146">
+        <v>373</v>
+      </c>
+      <c r="M146">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="147" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>245</v>
       </c>
@@ -7442,8 +7672,32 @@
       <c r="G147">
         <v>37</v>
       </c>
-    </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H147">
+        <f t="shared" ref="H147" si="18">I146</f>
+        <v>287</v>
+      </c>
+      <c r="I147">
+        <f t="shared" ref="I147" si="19">H146</f>
+        <v>476</v>
+      </c>
+      <c r="J147">
+        <f t="shared" ref="J147" si="20">K146</f>
+        <v>108</v>
+      </c>
+      <c r="K147">
+        <f t="shared" ref="K147" si="21">J146</f>
+        <v>103</v>
+      </c>
+      <c r="L147">
+        <f t="shared" ref="L147" si="22">M146</f>
+        <v>179</v>
+      </c>
+      <c r="M147">
+        <f t="shared" ref="M147" si="23">L146</f>
+        <v>373</v>
+      </c>
+    </row>
+    <row r="148" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>193</v>
       </c>
@@ -7465,8 +7719,26 @@
       <c r="G148">
         <v>0</v>
       </c>
-    </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H148">
+        <v>421</v>
+      </c>
+      <c r="I148">
+        <v>287</v>
+      </c>
+      <c r="J148">
+        <v>215</v>
+      </c>
+      <c r="K148">
+        <v>153</v>
+      </c>
+      <c r="L148">
+        <v>206</v>
+      </c>
+      <c r="M148">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="149" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>160</v>
       </c>
@@ -7488,8 +7760,32 @@
       <c r="G149">
         <v>27</v>
       </c>
-    </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H149">
+        <f t="shared" ref="H149" si="24">I148</f>
+        <v>287</v>
+      </c>
+      <c r="I149">
+        <f t="shared" ref="I149" si="25">H148</f>
+        <v>421</v>
+      </c>
+      <c r="J149">
+        <f t="shared" ref="J149" si="26">K148</f>
+        <v>153</v>
+      </c>
+      <c r="K149">
+        <f t="shared" ref="K149" si="27">J148</f>
+        <v>215</v>
+      </c>
+      <c r="L149">
+        <f t="shared" ref="L149" si="28">M148</f>
+        <v>134</v>
+      </c>
+      <c r="M149">
+        <f t="shared" ref="M149" si="29">L148</f>
+        <v>206</v>
+      </c>
+    </row>
+    <row r="150" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>36</v>
       </c>
@@ -7511,8 +7807,26 @@
       <c r="G150">
         <v>20</v>
       </c>
-    </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H150">
+        <v>503</v>
+      </c>
+      <c r="I150">
+        <v>360</v>
+      </c>
+      <c r="J150">
+        <v>282</v>
+      </c>
+      <c r="K150">
+        <v>92</v>
+      </c>
+      <c r="L150">
+        <v>221</v>
+      </c>
+      <c r="M150">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>246</v>
       </c>
@@ -7534,8 +7848,32 @@
       <c r="G151">
         <v>38</v>
       </c>
-    </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H151">
+        <f t="shared" ref="H151" si="30">I150</f>
+        <v>360</v>
+      </c>
+      <c r="I151">
+        <f t="shared" ref="I151" si="31">H150</f>
+        <v>503</v>
+      </c>
+      <c r="J151">
+        <f t="shared" ref="J151" si="32">K150</f>
+        <v>92</v>
+      </c>
+      <c r="K151">
+        <f t="shared" ref="K151" si="33">J150</f>
+        <v>282</v>
+      </c>
+      <c r="L151">
+        <f t="shared" ref="L151" si="34">M150</f>
+        <v>268</v>
+      </c>
+      <c r="M151">
+        <f t="shared" ref="M151" si="35">L150</f>
+        <v>221</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>227</v>
       </c>
@@ -7557,8 +7895,26 @@
       <c r="G152">
         <v>35</v>
       </c>
-    </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H152">
+        <v>388</v>
+      </c>
+      <c r="I152">
+        <v>459</v>
+      </c>
+      <c r="J152">
+        <v>124</v>
+      </c>
+      <c r="K152">
+        <v>236</v>
+      </c>
+      <c r="L152">
+        <v>264</v>
+      </c>
+      <c r="M152">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>164</v>
       </c>
@@ -7580,8 +7936,32 @@
       <c r="G153">
         <v>32</v>
       </c>
-    </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H153">
+        <f t="shared" ref="H153" si="36">I152</f>
+        <v>459</v>
+      </c>
+      <c r="I153">
+        <f t="shared" ref="I153" si="37">H152</f>
+        <v>388</v>
+      </c>
+      <c r="J153">
+        <f t="shared" ref="J153" si="38">K152</f>
+        <v>236</v>
+      </c>
+      <c r="K153">
+        <f t="shared" ref="K153" si="39">J152</f>
+        <v>124</v>
+      </c>
+      <c r="L153">
+        <f t="shared" ref="L153" si="40">M152</f>
+        <v>223</v>
+      </c>
+      <c r="M153">
+        <f t="shared" ref="M153" si="41">L152</f>
+        <v>264</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>37</v>
       </c>
@@ -7603,8 +7983,26 @@
       <c r="G154">
         <v>18</v>
       </c>
-    </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H154">
+        <v>490</v>
+      </c>
+      <c r="I154">
+        <v>313</v>
+      </c>
+      <c r="J154">
+        <v>132</v>
+      </c>
+      <c r="K154">
+        <v>138</v>
+      </c>
+      <c r="L154">
+        <v>358</v>
+      </c>
+      <c r="M154">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="155" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>177</v>
       </c>
@@ -7626,8 +8024,32 @@
       <c r="G155">
         <v>49</v>
       </c>
-    </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H155">
+        <f t="shared" ref="H155" si="42">I154</f>
+        <v>313</v>
+      </c>
+      <c r="I155">
+        <f t="shared" ref="I155" si="43">H154</f>
+        <v>490</v>
+      </c>
+      <c r="J155">
+        <f t="shared" ref="J155" si="44">K154</f>
+        <v>138</v>
+      </c>
+      <c r="K155">
+        <f t="shared" ref="K155" si="45">J154</f>
+        <v>132</v>
+      </c>
+      <c r="L155">
+        <f t="shared" ref="L155" si="46">M154</f>
+        <v>175</v>
+      </c>
+      <c r="M155">
+        <f t="shared" ref="M155" si="47">L154</f>
+        <v>358</v>
+      </c>
+    </row>
+    <row r="156" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>130</v>
       </c>
@@ -7649,8 +8071,26 @@
       <c r="G156">
         <v>34</v>
       </c>
-    </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H156">
+        <v>529</v>
+      </c>
+      <c r="I156">
+        <v>378</v>
+      </c>
+      <c r="J156">
+        <v>201</v>
+      </c>
+      <c r="K156">
+        <v>207</v>
+      </c>
+      <c r="L156">
+        <v>328</v>
+      </c>
+      <c r="M156">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="157" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>63</v>
       </c>
@@ -7672,8 +8112,32 @@
       <c r="G157">
         <v>37</v>
       </c>
-    </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H157">
+        <f t="shared" ref="H157" si="48">I156</f>
+        <v>378</v>
+      </c>
+      <c r="I157">
+        <f t="shared" ref="I157" si="49">H156</f>
+        <v>529</v>
+      </c>
+      <c r="J157">
+        <f t="shared" ref="J157" si="50">K156</f>
+        <v>207</v>
+      </c>
+      <c r="K157">
+        <f t="shared" ref="K157" si="51">J156</f>
+        <v>201</v>
+      </c>
+      <c r="L157">
+        <f t="shared" ref="L157" si="52">M156</f>
+        <v>171</v>
+      </c>
+      <c r="M157">
+        <f t="shared" ref="M157" si="53">L156</f>
+        <v>328</v>
+      </c>
+    </row>
+    <row r="158" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>21</v>
       </c>
@@ -7695,8 +8159,26 @@
       <c r="G158">
         <v>14</v>
       </c>
-    </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H158">
+        <v>592</v>
+      </c>
+      <c r="I158">
+        <v>320</v>
+      </c>
+      <c r="J158">
+        <v>507</v>
+      </c>
+      <c r="K158">
+        <v>90</v>
+      </c>
+      <c r="L158">
+        <v>85</v>
+      </c>
+      <c r="M158">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="159" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>76</v>
       </c>
@@ -7718,8 +8200,32 @@
       <c r="G159">
         <v>70</v>
       </c>
-    </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H159">
+        <f t="shared" ref="H159" si="54">I158</f>
+        <v>320</v>
+      </c>
+      <c r="I159">
+        <f t="shared" ref="I159" si="55">H158</f>
+        <v>592</v>
+      </c>
+      <c r="J159">
+        <f t="shared" ref="J159" si="56">K158</f>
+        <v>90</v>
+      </c>
+      <c r="K159">
+        <f t="shared" ref="K159" si="57">J158</f>
+        <v>507</v>
+      </c>
+      <c r="L159">
+        <f t="shared" ref="L159" si="58">M158</f>
+        <v>230</v>
+      </c>
+      <c r="M159">
+        <f t="shared" ref="M159" si="59">L158</f>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="160" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>33</v>
       </c>
@@ -7741,8 +8247,26 @@
       <c r="G160">
         <v>42</v>
       </c>
-    </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H160">
+        <v>376</v>
+      </c>
+      <c r="I160">
+        <v>433</v>
+      </c>
+      <c r="J160">
+        <v>102</v>
+      </c>
+      <c r="K160">
+        <v>113</v>
+      </c>
+      <c r="L160">
+        <v>274</v>
+      </c>
+      <c r="M160">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="161" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>228</v>
       </c>
@@ -7764,8 +8288,32 @@
       <c r="G161">
         <v>32</v>
       </c>
-    </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H161">
+        <f t="shared" ref="H161" si="60">I160</f>
+        <v>433</v>
+      </c>
+      <c r="I161">
+        <f t="shared" ref="I161" si="61">H160</f>
+        <v>376</v>
+      </c>
+      <c r="J161">
+        <f t="shared" ref="J161" si="62">K160</f>
+        <v>113</v>
+      </c>
+      <c r="K161">
+        <f t="shared" ref="K161" si="63">J160</f>
+        <v>102</v>
+      </c>
+      <c r="L161">
+        <f t="shared" ref="L161" si="64">M160</f>
+        <v>320</v>
+      </c>
+      <c r="M161">
+        <f t="shared" ref="M161" si="65">L160</f>
+        <v>274</v>
+      </c>
+    </row>
+    <row r="162" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>73</v>
       </c>
@@ -7787,8 +8335,26 @@
       <c r="G162">
         <v>31</v>
       </c>
-    </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H162">
+        <v>226</v>
+      </c>
+      <c r="I162">
+        <v>453</v>
+      </c>
+      <c r="J162">
+        <v>58</v>
+      </c>
+      <c r="K162">
+        <v>168</v>
+      </c>
+      <c r="L162">
+        <v>168</v>
+      </c>
+      <c r="M162">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="163" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>68</v>
       </c>
@@ -7810,1201 +8376,2229 @@
       <c r="G163">
         <v>14</v>
       </c>
-    </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H163">
+        <f t="shared" ref="H163" si="66">I162</f>
+        <v>453</v>
+      </c>
+      <c r="I163">
+        <f t="shared" ref="I163" si="67">H162</f>
+        <v>226</v>
+      </c>
+      <c r="J163">
+        <f t="shared" ref="J163" si="68">K162</f>
+        <v>168</v>
+      </c>
+      <c r="K163">
+        <f t="shared" ref="K163" si="69">J162</f>
+        <v>58</v>
+      </c>
+      <c r="L163">
+        <f t="shared" ref="L163" si="70">M162</f>
+        <v>285</v>
+      </c>
+      <c r="M163">
+        <f t="shared" ref="M163" si="71">L162</f>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="164" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B164" t="s">
-        <v>66</v>
+        <v>216</v>
       </c>
       <c r="C164">
         <v>2018</v>
       </c>
       <c r="D164" t="s">
-        <v>92</v>
+        <v>142</v>
       </c>
       <c r="E164" t="s">
-        <v>166</v>
+        <v>69</v>
       </c>
       <c r="F164">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="G164">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="H164">
+        <v>392</v>
+      </c>
+      <c r="I164">
+        <v>283</v>
+      </c>
+      <c r="J164">
+        <v>260</v>
+      </c>
+      <c r="K164">
+        <v>206</v>
+      </c>
+      <c r="L164">
+        <v>132</v>
+      </c>
+      <c r="M164">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="165" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>166</v>
+        <v>247</v>
       </c>
       <c r="B165" t="s">
-        <v>203</v>
+        <v>238</v>
       </c>
       <c r="C165">
         <v>2018</v>
       </c>
       <c r="D165" t="s">
-        <v>92</v>
+        <v>142</v>
       </c>
       <c r="E165" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F165">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G165">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="H165">
+        <f t="shared" ref="H165:H196" si="72">I164</f>
+        <v>283</v>
+      </c>
+      <c r="I165">
+        <f t="shared" ref="I165:I196" si="73">H164</f>
+        <v>392</v>
+      </c>
+      <c r="J165">
+        <f t="shared" ref="J165:J196" si="74">K164</f>
+        <v>206</v>
+      </c>
+      <c r="K165">
+        <f t="shared" ref="K165:K196" si="75">J164</f>
+        <v>260</v>
+      </c>
+      <c r="L165">
+        <f t="shared" ref="L165:L196" si="76">M164</f>
+        <v>77</v>
+      </c>
+      <c r="M165">
+        <f t="shared" ref="M165:M196" si="77">L164</f>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="166" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>189</v>
+        <v>229</v>
       </c>
       <c r="B166" t="s">
-        <v>216</v>
+        <v>239</v>
       </c>
       <c r="C166">
         <v>2018</v>
       </c>
       <c r="D166" t="s">
-        <v>142</v>
+        <v>224</v>
       </c>
       <c r="E166" t="s">
-        <v>69</v>
+        <v>248</v>
       </c>
       <c r="F166">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="G166">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="H166">
+        <v>290</v>
+      </c>
+      <c r="I166">
+        <v>264</v>
+      </c>
+      <c r="J166">
+        <v>262</v>
+      </c>
+      <c r="K166">
+        <v>100</v>
+      </c>
+      <c r="L166">
+        <v>28</v>
+      </c>
+      <c r="M166">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="167" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B167" t="s">
-        <v>238</v>
+        <v>249</v>
       </c>
       <c r="C167">
         <v>2018</v>
       </c>
       <c r="D167" t="s">
-        <v>142</v>
+        <v>224</v>
       </c>
       <c r="E167" t="s">
-        <v>189</v>
+        <v>229</v>
       </c>
       <c r="F167">
+        <v>7</v>
+      </c>
+      <c r="G167">
         <v>10</v>
       </c>
-      <c r="G167">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H167">
+        <f t="shared" ref="H167:H213" si="78">I166</f>
+        <v>264</v>
+      </c>
+      <c r="I167">
+        <f t="shared" ref="I167:I213" si="79">H166</f>
+        <v>290</v>
+      </c>
+      <c r="J167">
+        <f t="shared" ref="J167:J213" si="80">K166</f>
+        <v>100</v>
+      </c>
+      <c r="K167">
+        <f t="shared" ref="K167:K213" si="81">J166</f>
+        <v>262</v>
+      </c>
+      <c r="L167">
+        <f t="shared" ref="L167:L213" si="82">M166</f>
+        <v>164</v>
+      </c>
+      <c r="M167">
+        <f t="shared" ref="M167:M213" si="83">L166</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="168" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>229</v>
+        <v>171</v>
       </c>
       <c r="B168" t="s">
-        <v>239</v>
+        <v>61</v>
       </c>
       <c r="C168">
         <v>2018</v>
       </c>
       <c r="D168" t="s">
-        <v>224</v>
+        <v>141</v>
       </c>
       <c r="E168" t="s">
-        <v>248</v>
+        <v>230</v>
       </c>
       <c r="F168">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="G168">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+      <c r="H168">
+        <v>281</v>
+      </c>
+      <c r="I168">
+        <v>563</v>
+      </c>
+      <c r="J168">
+        <v>53</v>
+      </c>
+      <c r="K168">
+        <v>123</v>
+      </c>
+      <c r="L168">
+        <v>228</v>
+      </c>
+      <c r="M168">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="169" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>248</v>
+        <v>230</v>
       </c>
       <c r="B169" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="C169">
         <v>2018</v>
       </c>
       <c r="D169" t="s">
-        <v>224</v>
+        <v>141</v>
       </c>
       <c r="E169" t="s">
-        <v>229</v>
+        <v>171</v>
       </c>
       <c r="F169">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="G169">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="H169">
+        <f t="shared" ref="H169:H213" si="84">I168</f>
+        <v>563</v>
+      </c>
+      <c r="I169">
+        <f t="shared" ref="I169:I213" si="85">H168</f>
+        <v>281</v>
+      </c>
+      <c r="J169">
+        <f t="shared" ref="J169:J213" si="86">K168</f>
+        <v>123</v>
+      </c>
+      <c r="K169">
+        <f t="shared" ref="K169:K213" si="87">J168</f>
+        <v>53</v>
+      </c>
+      <c r="L169">
+        <f t="shared" ref="L169:L213" si="88">M168</f>
+        <v>440</v>
+      </c>
+      <c r="M169">
+        <f t="shared" ref="M169:M213" si="89">L168</f>
+        <v>228</v>
+      </c>
+    </row>
+    <row r="170" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>171</v>
+        <v>95</v>
       </c>
       <c r="B170" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="C170">
         <v>2018</v>
       </c>
       <c r="D170" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="E170" t="s">
-        <v>230</v>
+        <v>133</v>
       </c>
       <c r="F170">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="G170">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="H170">
+        <v>169</v>
+      </c>
+      <c r="I170">
+        <v>406</v>
+      </c>
+      <c r="J170">
+        <v>121</v>
+      </c>
+      <c r="K170">
+        <v>333</v>
+      </c>
+      <c r="L170">
+        <v>48</v>
+      </c>
+      <c r="M170">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="171" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>230</v>
+        <v>133</v>
       </c>
       <c r="B171" t="s">
-        <v>240</v>
+        <v>135</v>
       </c>
       <c r="C171">
         <v>2018</v>
       </c>
       <c r="D171" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="E171" t="s">
-        <v>171</v>
+        <v>95</v>
       </c>
       <c r="F171">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="G171">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="H171">
+        <f t="shared" ref="H171:H213" si="90">I170</f>
+        <v>406</v>
+      </c>
+      <c r="I171">
+        <f t="shared" ref="I171:I213" si="91">H170</f>
+        <v>169</v>
+      </c>
+      <c r="J171">
+        <f t="shared" ref="J171:J213" si="92">K170</f>
+        <v>333</v>
+      </c>
+      <c r="K171">
+        <f t="shared" ref="K171:K213" si="93">J170</f>
+        <v>121</v>
+      </c>
+      <c r="L171">
+        <f t="shared" ref="L171:L213" si="94">M170</f>
+        <v>73</v>
+      </c>
+      <c r="M171">
+        <f t="shared" ref="M171:M213" si="95">L170</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="172" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>95</v>
+        <v>190</v>
       </c>
       <c r="B172" t="s">
-        <v>96</v>
+        <v>217</v>
       </c>
       <c r="C172">
         <v>2018</v>
       </c>
       <c r="D172" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E172" t="s">
-        <v>133</v>
+        <v>231</v>
       </c>
       <c r="F172">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="G172">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="H172">
+        <v>668</v>
+      </c>
+      <c r="I172">
+        <v>573</v>
+      </c>
+      <c r="J172">
+        <v>284</v>
+      </c>
+      <c r="K172">
+        <v>287</v>
+      </c>
+      <c r="L172">
+        <v>384</v>
+      </c>
+      <c r="M172">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="173" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>133</v>
+        <v>231</v>
       </c>
       <c r="B173" t="s">
-        <v>135</v>
+        <v>241</v>
       </c>
       <c r="C173">
         <v>2018</v>
       </c>
       <c r="D173" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E173" t="s">
-        <v>95</v>
+        <v>190</v>
       </c>
       <c r="F173">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G173">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+      <c r="H173">
+        <f t="shared" ref="H173:H213" si="96">I172</f>
+        <v>573</v>
+      </c>
+      <c r="I173">
+        <f t="shared" ref="I173:I213" si="97">H172</f>
+        <v>668</v>
+      </c>
+      <c r="J173">
+        <f t="shared" ref="J173:J213" si="98">K172</f>
+        <v>287</v>
+      </c>
+      <c r="K173">
+        <f t="shared" ref="K173:K213" si="99">J172</f>
+        <v>284</v>
+      </c>
+      <c r="L173">
+        <f t="shared" ref="L173:L213" si="100">M172</f>
+        <v>286</v>
+      </c>
+      <c r="M173">
+        <f t="shared" ref="M173:M213" si="101">L172</f>
+        <v>384</v>
+      </c>
+    </row>
+    <row r="174" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>190</v>
+        <v>25</v>
       </c>
       <c r="B174" t="s">
-        <v>217</v>
+        <v>26</v>
       </c>
       <c r="C174">
         <v>2018</v>
       </c>
       <c r="D174" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="E174" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="F174">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="G174">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="H174">
+        <v>586</v>
+      </c>
+      <c r="I174">
+        <v>263</v>
+      </c>
+      <c r="J174">
+        <v>208</v>
+      </c>
+      <c r="K174">
+        <v>79</v>
+      </c>
+      <c r="L174">
+        <v>378</v>
+      </c>
+      <c r="M174">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="175" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B175" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C175">
         <v>2018</v>
       </c>
       <c r="D175" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="E175" t="s">
-        <v>190</v>
+        <v>25</v>
       </c>
       <c r="F175">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="G175">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+      <c r="H175">
+        <f t="shared" ref="H175:H213" si="102">I174</f>
+        <v>263</v>
+      </c>
+      <c r="I175">
+        <f t="shared" ref="I175:I213" si="103">H174</f>
+        <v>586</v>
+      </c>
+      <c r="J175">
+        <f t="shared" ref="J175:J213" si="104">K174</f>
+        <v>79</v>
+      </c>
+      <c r="K175">
+        <f t="shared" ref="K175:K213" si="105">J174</f>
+        <v>208</v>
+      </c>
+      <c r="L175">
+        <f t="shared" ref="L175:L213" si="106">M174</f>
+        <v>184</v>
+      </c>
+      <c r="M175">
+        <f t="shared" ref="M175:M213" si="107">L174</f>
+        <v>378</v>
+      </c>
+    </row>
+    <row r="176" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B176" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C176">
         <v>2018</v>
       </c>
       <c r="D176" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E176" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F176">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="G176">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="H176">
+        <v>423</v>
+      </c>
+      <c r="I176">
+        <v>416</v>
+      </c>
+      <c r="J176">
+        <v>146</v>
+      </c>
+      <c r="K176">
+        <v>113</v>
+      </c>
+      <c r="L176">
+        <v>277</v>
+      </c>
+      <c r="M176">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="177" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B177" t="s">
-        <v>242</v>
+        <v>222</v>
       </c>
       <c r="C177">
         <v>2018</v>
       </c>
       <c r="D177" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E177" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F177">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="G177">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="H177">
+        <f t="shared" ref="H177:H213" si="108">I176</f>
+        <v>416</v>
+      </c>
+      <c r="I177">
+        <f t="shared" ref="I177:I213" si="109">H176</f>
+        <v>423</v>
+      </c>
+      <c r="J177">
+        <f t="shared" ref="J177:J213" si="110">K176</f>
+        <v>113</v>
+      </c>
+      <c r="K177">
+        <f t="shared" ref="K177:K213" si="111">J176</f>
+        <v>146</v>
+      </c>
+      <c r="L177">
+        <f t="shared" ref="L177:L213" si="112">M176</f>
+        <v>303</v>
+      </c>
+      <c r="M177">
+        <f t="shared" ref="M177:M213" si="113">L176</f>
+        <v>277</v>
+      </c>
+    </row>
+    <row r="178" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>24</v>
+        <v>81</v>
       </c>
       <c r="B178" t="s">
-        <v>18</v>
+        <v>82</v>
       </c>
       <c r="C178">
         <v>2018</v>
       </c>
       <c r="D178" t="s">
-        <v>147</v>
+        <v>54</v>
       </c>
       <c r="E178" t="s">
-        <v>233</v>
+        <v>169</v>
       </c>
       <c r="F178">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="G178">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="H178">
+        <v>515</v>
+      </c>
+      <c r="I178">
+        <v>327</v>
+      </c>
+      <c r="J178">
+        <v>200</v>
+      </c>
+      <c r="K178">
+        <v>28</v>
+      </c>
+      <c r="L178">
+        <v>315</v>
+      </c>
+      <c r="M178">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="179" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>233</v>
+        <v>169</v>
       </c>
       <c r="B179" t="s">
-        <v>222</v>
+        <v>38</v>
       </c>
       <c r="C179">
         <v>2018</v>
       </c>
       <c r="D179" t="s">
-        <v>147</v>
+        <v>54</v>
       </c>
       <c r="E179" t="s">
-        <v>24</v>
+        <v>81</v>
       </c>
       <c r="F179">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G179">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="H179">
+        <f t="shared" ref="H179:H213" si="114">I178</f>
+        <v>327</v>
+      </c>
+      <c r="I179">
+        <f t="shared" ref="I179:I213" si="115">H178</f>
+        <v>515</v>
+      </c>
+      <c r="J179">
+        <f t="shared" ref="J179:J213" si="116">K178</f>
+        <v>28</v>
+      </c>
+      <c r="K179">
+        <f t="shared" ref="K179:K213" si="117">J178</f>
+        <v>200</v>
+      </c>
+      <c r="L179">
+        <f t="shared" ref="L179:L213" si="118">M178</f>
+        <v>299</v>
+      </c>
+      <c r="M179">
+        <f t="shared" ref="M179:M213" si="119">L178</f>
+        <v>315</v>
+      </c>
+    </row>
+    <row r="180" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="B180" t="s">
-        <v>82</v>
+        <v>113</v>
       </c>
       <c r="C180">
         <v>2018</v>
       </c>
       <c r="D180" t="s">
-        <v>54</v>
+        <v>148</v>
       </c>
       <c r="E180" t="s">
-        <v>169</v>
+        <v>45</v>
       </c>
       <c r="F180">
+        <v>3</v>
+      </c>
+      <c r="G180">
+        <v>30</v>
+      </c>
+      <c r="H180">
+        <v>248</v>
+      </c>
+      <c r="I180">
+        <v>538</v>
+      </c>
+      <c r="J180">
+        <v>88</v>
+      </c>
+      <c r="K180">
+        <v>211</v>
+      </c>
+      <c r="L180">
+        <v>160</v>
+      </c>
+      <c r="M180">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="181" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>45</v>
+      </c>
+      <c r="B181" t="s">
         <v>26</v>
-      </c>
-      <c r="G180">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A181" t="s">
-        <v>169</v>
-      </c>
-      <c r="B181" t="s">
-        <v>38</v>
       </c>
       <c r="C181">
         <v>2018</v>
       </c>
       <c r="D181" t="s">
-        <v>54</v>
+        <v>148</v>
       </c>
       <c r="E181" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="F181">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G181">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="H181">
+        <f t="shared" ref="H181:H213" si="120">I180</f>
+        <v>538</v>
+      </c>
+      <c r="I181">
+        <f t="shared" ref="I181:I213" si="121">H180</f>
+        <v>248</v>
+      </c>
+      <c r="J181">
+        <f t="shared" ref="J181:J213" si="122">K180</f>
+        <v>211</v>
+      </c>
+      <c r="K181">
+        <f t="shared" ref="K181:K213" si="123">J180</f>
+        <v>88</v>
+      </c>
+      <c r="L181">
+        <f t="shared" ref="L181:L213" si="124">M180</f>
+        <v>327</v>
+      </c>
+      <c r="M181">
+        <f t="shared" ref="M181:M213" si="125">L180</f>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="182" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B182" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="C182">
         <v>2018</v>
       </c>
       <c r="D182" t="s">
-        <v>148</v>
+        <v>110</v>
       </c>
       <c r="E182" t="s">
+        <v>59</v>
+      </c>
+      <c r="F182">
         <v>45</v>
       </c>
-      <c r="F182">
-        <v>3</v>
-      </c>
       <c r="G182">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="H182">
+        <v>528</v>
+      </c>
+      <c r="I182">
+        <v>471</v>
+      </c>
+      <c r="J182">
+        <v>200</v>
+      </c>
+      <c r="K182">
+        <v>163</v>
+      </c>
+      <c r="L182">
+        <v>328</v>
+      </c>
+      <c r="M182">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="183" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="B183" t="s">
-        <v>26</v>
+        <v>115</v>
       </c>
       <c r="C183">
         <v>2018</v>
       </c>
       <c r="D183" t="s">
-        <v>148</v>
+        <v>110</v>
       </c>
       <c r="E183" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F183">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G183">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+      <c r="H183">
+        <f t="shared" ref="H183:H213" si="126">I182</f>
+        <v>471</v>
+      </c>
+      <c r="I183">
+        <f t="shared" ref="I183:I213" si="127">H182</f>
+        <v>528</v>
+      </c>
+      <c r="J183">
+        <f t="shared" ref="J183:J213" si="128">K182</f>
+        <v>163</v>
+      </c>
+      <c r="K183">
+        <f t="shared" ref="K183:K213" si="129">J182</f>
+        <v>200</v>
+      </c>
+      <c r="L183">
+        <f t="shared" ref="L183:L213" si="130">M182</f>
+        <v>308</v>
+      </c>
+      <c r="M183">
+        <f t="shared" ref="M183:M213" si="131">L182</f>
+        <v>328</v>
+      </c>
+    </row>
+    <row r="184" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>13</v>
+        <v>188</v>
       </c>
       <c r="B184" t="s">
-        <v>14</v>
+        <v>215</v>
       </c>
       <c r="C184">
         <v>2018</v>
       </c>
       <c r="D184" t="s">
-        <v>110</v>
+        <v>43</v>
       </c>
       <c r="E184" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F184">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="G184">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="H184">
+        <v>326</v>
+      </c>
+      <c r="I184">
+        <v>427</v>
+      </c>
+      <c r="J184">
+        <v>77</v>
+      </c>
+      <c r="K184">
+        <v>257</v>
+      </c>
+      <c r="L184">
+        <v>249</v>
+      </c>
+      <c r="M184">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="185" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B185" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="C185">
         <v>2018</v>
       </c>
       <c r="D185" t="s">
-        <v>110</v>
+        <v>43</v>
       </c>
       <c r="E185" t="s">
-        <v>13</v>
+        <v>188</v>
       </c>
       <c r="F185">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="G185">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="H185">
+        <f t="shared" ref="H185:H213" si="132">I184</f>
+        <v>427</v>
+      </c>
+      <c r="I185">
+        <f t="shared" ref="I185:I213" si="133">H184</f>
+        <v>326</v>
+      </c>
+      <c r="J185">
+        <f t="shared" ref="J185:J213" si="134">K184</f>
+        <v>257</v>
+      </c>
+      <c r="K185">
+        <f t="shared" ref="K185:K213" si="135">J184</f>
+        <v>77</v>
+      </c>
+      <c r="L185">
+        <f t="shared" ref="L185:L213" si="136">M184</f>
+        <v>170</v>
+      </c>
+      <c r="M185">
+        <f t="shared" ref="M185:M213" si="137">L184</f>
+        <v>249</v>
+      </c>
+    </row>
+    <row r="186" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>188</v>
+        <v>119</v>
       </c>
       <c r="B186" t="s">
-        <v>215</v>
+        <v>120</v>
       </c>
       <c r="C186">
         <v>2018</v>
       </c>
       <c r="D186" t="s">
-        <v>43</v>
+        <v>152</v>
       </c>
       <c r="E186" t="s">
-        <v>56</v>
+        <v>180</v>
       </c>
       <c r="F186">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="G186">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="H186">
+        <v>251</v>
+      </c>
+      <c r="I186">
+        <v>413</v>
+      </c>
+      <c r="J186">
+        <v>33</v>
+      </c>
+      <c r="K186">
+        <v>205</v>
+      </c>
+      <c r="L186">
+        <v>218</v>
+      </c>
+      <c r="M186">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="187" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>56</v>
+        <v>180</v>
       </c>
       <c r="B187" t="s">
-        <v>57</v>
+        <v>209</v>
       </c>
       <c r="C187">
         <v>2018</v>
       </c>
       <c r="D187" t="s">
-        <v>43</v>
+        <v>152</v>
       </c>
       <c r="E187" t="s">
-        <v>188</v>
+        <v>119</v>
       </c>
       <c r="F187">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="G187">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="H187">
+        <f t="shared" ref="H187:H213" si="138">I186</f>
+        <v>413</v>
+      </c>
+      <c r="I187">
+        <f t="shared" ref="I187:I213" si="139">H186</f>
+        <v>251</v>
+      </c>
+      <c r="J187">
+        <f t="shared" ref="J187:J213" si="140">K186</f>
+        <v>205</v>
+      </c>
+      <c r="K187">
+        <f t="shared" ref="K187:K213" si="141">J186</f>
+        <v>33</v>
+      </c>
+      <c r="L187">
+        <f t="shared" ref="L187:L213" si="142">M186</f>
+        <v>208</v>
+      </c>
+      <c r="M187">
+        <f t="shared" ref="M187:M213" si="143">L186</f>
+        <v>218</v>
+      </c>
+    </row>
+    <row r="188" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="B188" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="C188">
         <v>2018</v>
       </c>
       <c r="D188" t="s">
-        <v>152</v>
+        <v>31</v>
       </c>
       <c r="E188" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="F188">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G188">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="H188">
+        <v>285</v>
+      </c>
+      <c r="I188">
+        <v>499</v>
+      </c>
+      <c r="J188">
+        <v>85</v>
+      </c>
+      <c r="K188">
+        <v>224</v>
+      </c>
+      <c r="L188">
+        <v>200</v>
+      </c>
+      <c r="M188">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="189" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="B189" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="C189">
         <v>2018</v>
       </c>
       <c r="D189" t="s">
-        <v>152</v>
+        <v>31</v>
       </c>
       <c r="E189" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="F189">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="G189">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="H189">
+        <f t="shared" ref="H189:H213" si="144">I188</f>
+        <v>499</v>
+      </c>
+      <c r="I189">
+        <f t="shared" ref="I189:I213" si="145">H188</f>
+        <v>285</v>
+      </c>
+      <c r="J189">
+        <f t="shared" ref="J189:J213" si="146">K188</f>
+        <v>224</v>
+      </c>
+      <c r="K189">
+        <f t="shared" ref="K189:K213" si="147">J188</f>
+        <v>85</v>
+      </c>
+      <c r="L189">
+        <f t="shared" ref="L189:L213" si="148">M188</f>
+        <v>275</v>
+      </c>
+      <c r="M189">
+        <f t="shared" ref="M189:M213" si="149">L188</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="190" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>104</v>
+        <v>41</v>
       </c>
       <c r="B190" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="C190">
         <v>2018</v>
       </c>
       <c r="D190" t="s">
+        <v>143</v>
+      </c>
+      <c r="E190" t="s">
+        <v>181</v>
+      </c>
+      <c r="F190">
+        <v>35</v>
+      </c>
+      <c r="G190">
         <v>31</v>
       </c>
-      <c r="E190" t="s">
-        <v>163</v>
-      </c>
-      <c r="F190">
-        <v>16</v>
-      </c>
-      <c r="G190">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H190">
+        <v>462</v>
+      </c>
+      <c r="I190">
+        <v>443</v>
+      </c>
+      <c r="J190">
+        <v>256</v>
+      </c>
+      <c r="K190">
+        <v>224</v>
+      </c>
+      <c r="L190">
+        <v>206</v>
+      </c>
+      <c r="M190">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="191" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>163</v>
+        <v>181</v>
       </c>
       <c r="B191" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="C191">
         <v>2018</v>
       </c>
       <c r="D191" t="s">
+        <v>143</v>
+      </c>
+      <c r="E191" t="s">
+        <v>41</v>
+      </c>
+      <c r="F191">
         <v>31</v>
       </c>
-      <c r="E191" t="s">
-        <v>104</v>
-      </c>
-      <c r="F191">
-        <v>13</v>
-      </c>
       <c r="G191">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="H191">
+        <f t="shared" ref="H191:H213" si="150">I190</f>
+        <v>443</v>
+      </c>
+      <c r="I191">
+        <f t="shared" ref="I191:I213" si="151">H190</f>
+        <v>462</v>
+      </c>
+      <c r="J191">
+        <f t="shared" ref="J191:J213" si="152">K190</f>
+        <v>224</v>
+      </c>
+      <c r="K191">
+        <f t="shared" ref="K191:K213" si="153">J190</f>
+        <v>256</v>
+      </c>
+      <c r="L191">
+        <f t="shared" ref="L191:L213" si="154">M190</f>
+        <v>219</v>
+      </c>
+      <c r="M191">
+        <f t="shared" ref="M191:M213" si="155">L190</f>
+        <v>206</v>
+      </c>
+    </row>
+    <row r="192" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>41</v>
+        <v>172</v>
       </c>
       <c r="B192" t="s">
-        <v>42</v>
+        <v>205</v>
       </c>
       <c r="C192">
         <v>2018</v>
       </c>
       <c r="D192" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="E192" t="s">
-        <v>181</v>
+        <v>84</v>
       </c>
       <c r="F192">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="G192">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="H192">
+        <v>331</v>
+      </c>
+      <c r="I192">
+        <v>203</v>
+      </c>
+      <c r="J192">
+        <v>159</v>
+      </c>
+      <c r="K192">
+        <v>37</v>
+      </c>
+      <c r="L192">
+        <v>172</v>
+      </c>
+      <c r="M192">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="193" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>181</v>
+        <v>84</v>
       </c>
       <c r="B193" t="s">
-        <v>210</v>
+        <v>117</v>
       </c>
       <c r="C193">
         <v>2018</v>
       </c>
       <c r="D193" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="E193" t="s">
-        <v>41</v>
+        <v>172</v>
       </c>
       <c r="F193">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="G193">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="H193">
+        <f t="shared" ref="H193:H213" si="156">I192</f>
+        <v>203</v>
+      </c>
+      <c r="I193">
+        <f t="shared" ref="I193:I213" si="157">H192</f>
+        <v>331</v>
+      </c>
+      <c r="J193">
+        <f t="shared" ref="J193:J213" si="158">K192</f>
+        <v>37</v>
+      </c>
+      <c r="K193">
+        <f t="shared" ref="K193:K213" si="159">J192</f>
+        <v>159</v>
+      </c>
+      <c r="L193">
+        <f t="shared" ref="L193:L213" si="160">M192</f>
+        <v>166</v>
+      </c>
+      <c r="M193">
+        <f t="shared" ref="M193:M213" si="161">L192</f>
+        <v>172</v>
+      </c>
+    </row>
+    <row r="194" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>172</v>
+        <v>234</v>
       </c>
       <c r="B194" t="s">
-        <v>205</v>
+        <v>26</v>
       </c>
       <c r="C194">
         <v>2018</v>
       </c>
       <c r="D194" t="s">
-        <v>150</v>
+        <v>23</v>
       </c>
       <c r="E194" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="F194">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="G194">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="H194">
+        <v>637</v>
+      </c>
+      <c r="I194">
+        <v>502</v>
+      </c>
+      <c r="J194">
+        <v>264</v>
+      </c>
+      <c r="K194">
+        <v>169</v>
+      </c>
+      <c r="L194">
+        <v>373</v>
+      </c>
+      <c r="M194">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="195" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="B195" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C195">
         <v>2018</v>
       </c>
       <c r="D195" t="s">
-        <v>150</v>
+        <v>23</v>
       </c>
       <c r="E195" t="s">
-        <v>172</v>
+        <v>234</v>
       </c>
       <c r="F195">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="G195">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+      <c r="H195">
+        <f t="shared" ref="H195:H213" si="162">I194</f>
+        <v>502</v>
+      </c>
+      <c r="I195">
+        <f t="shared" ref="I195:I213" si="163">H194</f>
+        <v>637</v>
+      </c>
+      <c r="J195">
+        <f t="shared" ref="J195:J213" si="164">K194</f>
+        <v>169</v>
+      </c>
+      <c r="K195">
+        <f t="shared" ref="K195:K213" si="165">J194</f>
+        <v>264</v>
+      </c>
+      <c r="L195">
+        <f t="shared" ref="L195:L213" si="166">M194</f>
+        <v>333</v>
+      </c>
+      <c r="M195">
+        <f t="shared" ref="M195:M213" si="167">L194</f>
+        <v>373</v>
+      </c>
+    </row>
+    <row r="196" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>234</v>
+        <v>28</v>
       </c>
       <c r="B196" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="C196">
         <v>2018</v>
       </c>
       <c r="D196" t="s">
-        <v>23</v>
+        <v>146</v>
       </c>
       <c r="E196" t="s">
-        <v>98</v>
+        <v>187</v>
       </c>
       <c r="F196">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G196">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="H196">
+        <v>322</v>
+      </c>
+      <c r="I196">
+        <v>393</v>
+      </c>
+      <c r="J196">
+        <v>81</v>
+      </c>
+      <c r="K196">
+        <v>91</v>
+      </c>
+      <c r="L196">
+        <v>241</v>
+      </c>
+      <c r="M196">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="197" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>98</v>
+        <v>187</v>
       </c>
       <c r="B197" t="s">
-        <v>116</v>
+        <v>214</v>
       </c>
       <c r="C197">
         <v>2018</v>
       </c>
       <c r="D197" t="s">
-        <v>23</v>
+        <v>146</v>
       </c>
       <c r="E197" t="s">
-        <v>234</v>
+        <v>28</v>
       </c>
       <c r="F197">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="G197">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="H197">
+        <f t="shared" ref="H197:H213" si="168">I196</f>
+        <v>393</v>
+      </c>
+      <c r="I197">
+        <f t="shared" ref="I197:I213" si="169">H196</f>
+        <v>322</v>
+      </c>
+      <c r="J197">
+        <f t="shared" ref="J197:J213" si="170">K196</f>
+        <v>91</v>
+      </c>
+      <c r="K197">
+        <f t="shared" ref="K197:K213" si="171">J196</f>
+        <v>81</v>
+      </c>
+      <c r="L197">
+        <f t="shared" ref="L197:L213" si="172">M196</f>
+        <v>302</v>
+      </c>
+      <c r="M197">
+        <f t="shared" ref="M197:M213" si="173">L196</f>
+        <v>241</v>
+      </c>
+    </row>
+    <row r="198" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>28</v>
+        <v>111</v>
       </c>
       <c r="B198" t="s">
-        <v>86</v>
+        <v>124</v>
       </c>
       <c r="C198">
         <v>2018</v>
       </c>
       <c r="D198" t="s">
-        <v>146</v>
+        <v>225</v>
       </c>
       <c r="E198" t="s">
-        <v>187</v>
+        <v>88</v>
       </c>
       <c r="F198">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="G198">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="H198">
+        <v>541</v>
+      </c>
+      <c r="I198">
+        <v>273</v>
+      </c>
+      <c r="J198">
+        <v>401</v>
+      </c>
+      <c r="K198">
+        <v>134</v>
+      </c>
+      <c r="L198">
+        <v>140</v>
+      </c>
+      <c r="M198">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="199" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>187</v>
+        <v>88</v>
       </c>
       <c r="B199" t="s">
-        <v>214</v>
+        <v>103</v>
       </c>
       <c r="C199">
         <v>2018</v>
       </c>
       <c r="D199" t="s">
-        <v>146</v>
+        <v>225</v>
       </c>
       <c r="E199" t="s">
-        <v>28</v>
+        <v>111</v>
       </c>
       <c r="F199">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="G199">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+      <c r="H199">
+        <f t="shared" ref="H199:H213" si="174">I198</f>
+        <v>273</v>
+      </c>
+      <c r="I199">
+        <f t="shared" ref="I199:I213" si="175">H198</f>
+        <v>541</v>
+      </c>
+      <c r="J199">
+        <f t="shared" ref="J199:J213" si="176">K198</f>
+        <v>134</v>
+      </c>
+      <c r="K199">
+        <f t="shared" ref="K199:K213" si="177">J198</f>
+        <v>401</v>
+      </c>
+      <c r="L199">
+        <f t="shared" ref="L199:L213" si="178">M198</f>
+        <v>139</v>
+      </c>
+      <c r="M199">
+        <f t="shared" ref="M199:M213" si="179">L198</f>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="200" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>111</v>
+        <v>168</v>
       </c>
       <c r="B200" t="s">
-        <v>124</v>
+        <v>70</v>
       </c>
       <c r="C200">
         <v>2018</v>
       </c>
       <c r="D200" t="s">
-        <v>225</v>
+        <v>153</v>
       </c>
       <c r="E200" t="s">
-        <v>88</v>
+        <v>235</v>
       </c>
       <c r="F200">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="G200">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="H200">
+        <v>344</v>
+      </c>
+      <c r="I200">
+        <v>208</v>
+      </c>
+      <c r="J200">
+        <v>208</v>
+      </c>
+      <c r="K200">
+        <v>103</v>
+      </c>
+      <c r="L200">
+        <v>136</v>
+      </c>
+      <c r="M200">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="201" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>88</v>
+        <v>235</v>
       </c>
       <c r="B201" t="s">
-        <v>103</v>
+        <v>243</v>
       </c>
       <c r="C201">
         <v>2018</v>
       </c>
       <c r="D201" t="s">
-        <v>225</v>
+        <v>153</v>
       </c>
       <c r="E201" t="s">
-        <v>111</v>
+        <v>168</v>
       </c>
       <c r="F201">
+        <v>14</v>
+      </c>
+      <c r="G201">
         <v>13</v>
       </c>
-      <c r="G201">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H201">
+        <f t="shared" ref="H201:H213" si="180">I200</f>
+        <v>208</v>
+      </c>
+      <c r="I201">
+        <f t="shared" ref="I201:I213" si="181">H200</f>
+        <v>344</v>
+      </c>
+      <c r="J201">
+        <f t="shared" ref="J201:J213" si="182">K200</f>
+        <v>103</v>
+      </c>
+      <c r="K201">
+        <f t="shared" ref="K201:K213" si="183">J200</f>
+        <v>208</v>
+      </c>
+      <c r="L201">
+        <f t="shared" ref="L201:L213" si="184">M200</f>
+        <v>105</v>
+      </c>
+      <c r="M201">
+        <f t="shared" ref="M201:M213" si="185">L200</f>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="202" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>168</v>
+        <v>55</v>
       </c>
       <c r="B202" t="s">
-        <v>70</v>
+        <v>123</v>
       </c>
       <c r="C202">
         <v>2018</v>
       </c>
       <c r="D202" t="s">
-        <v>153</v>
+        <v>46</v>
       </c>
       <c r="E202" t="s">
-        <v>235</v>
+        <v>44</v>
       </c>
       <c r="F202">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="G202">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="H202">
+        <v>355</v>
+      </c>
+      <c r="I202">
+        <v>284</v>
+      </c>
+      <c r="J202">
+        <v>178</v>
+      </c>
+      <c r="K202">
+        <v>72</v>
+      </c>
+      <c r="L202">
+        <v>177</v>
+      </c>
+      <c r="M202">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="203" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>235</v>
+        <v>44</v>
       </c>
       <c r="B203" t="s">
-        <v>243</v>
+        <v>64</v>
       </c>
       <c r="C203">
         <v>2018</v>
       </c>
       <c r="D203" t="s">
-        <v>153</v>
+        <v>46</v>
       </c>
       <c r="E203" t="s">
-        <v>168</v>
+        <v>55</v>
       </c>
       <c r="F203">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="G203">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="H203">
+        <f t="shared" ref="H203:H213" si="186">I202</f>
+        <v>284</v>
+      </c>
+      <c r="I203">
+        <f t="shared" ref="I203:I213" si="187">H202</f>
+        <v>355</v>
+      </c>
+      <c r="J203">
+        <f t="shared" ref="J203:J213" si="188">K202</f>
+        <v>72</v>
+      </c>
+      <c r="K203">
+        <f t="shared" ref="K203:K213" si="189">J202</f>
+        <v>178</v>
+      </c>
+      <c r="L203">
+        <f t="shared" ref="L203:L213" si="190">M202</f>
+        <v>212</v>
+      </c>
+      <c r="M203">
+        <f t="shared" ref="M203:M213" si="191">L202</f>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="204" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>55</v>
+        <v>176</v>
       </c>
       <c r="B204" t="s">
-        <v>123</v>
+        <v>26</v>
       </c>
       <c r="C204">
         <v>2018</v>
       </c>
       <c r="D204" t="s">
-        <v>46</v>
+        <v>83</v>
       </c>
       <c r="E204" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F204">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="G204">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="H204">
+        <v>555</v>
+      </c>
+      <c r="I204">
+        <v>250</v>
+      </c>
+      <c r="J204">
+        <v>161</v>
+      </c>
+      <c r="K204">
+        <v>130</v>
+      </c>
+      <c r="L204">
+        <v>394</v>
+      </c>
+      <c r="M204">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="205" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B205" t="s">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="C205">
         <v>2018</v>
       </c>
       <c r="D205" t="s">
-        <v>46</v>
+        <v>83</v>
       </c>
       <c r="E205" t="s">
-        <v>55</v>
+        <v>176</v>
       </c>
       <c r="F205">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="G205">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="H205">
+        <f t="shared" ref="H205:H213" si="192">I204</f>
+        <v>250</v>
+      </c>
+      <c r="I205">
+        <f t="shared" ref="I205:I213" si="193">H204</f>
+        <v>555</v>
+      </c>
+      <c r="J205">
+        <f t="shared" ref="J205:J213" si="194">K204</f>
+        <v>130</v>
+      </c>
+      <c r="K205">
+        <f t="shared" ref="K205:K213" si="195">J204</f>
+        <v>161</v>
+      </c>
+      <c r="L205">
+        <f t="shared" ref="L205:L213" si="196">M204</f>
+        <v>120</v>
+      </c>
+      <c r="M205">
+        <f t="shared" ref="M205:M213" si="197">L204</f>
+        <v>394</v>
+      </c>
+    </row>
+    <row r="206" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>176</v>
+        <v>47</v>
       </c>
       <c r="B206" t="s">
-        <v>26</v>
+        <v>114</v>
       </c>
       <c r="C206">
         <v>2018</v>
       </c>
       <c r="D206" t="s">
-        <v>83</v>
+        <v>15</v>
       </c>
       <c r="E206" t="s">
-        <v>40</v>
+        <v>165</v>
       </c>
       <c r="F206">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="G206">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="H206">
+        <v>364</v>
+      </c>
+      <c r="I206">
+        <v>444</v>
+      </c>
+      <c r="J206">
+        <v>113</v>
+      </c>
+      <c r="K206">
+        <v>129</v>
+      </c>
+      <c r="L206">
+        <v>251</v>
+      </c>
+      <c r="M206">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="207" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>40</v>
+        <v>165</v>
       </c>
       <c r="B207" t="s">
-        <v>128</v>
+        <v>202</v>
       </c>
       <c r="C207">
         <v>2018</v>
       </c>
       <c r="D207" t="s">
-        <v>83</v>
+        <v>15</v>
       </c>
       <c r="E207" t="s">
-        <v>176</v>
+        <v>47</v>
       </c>
       <c r="F207">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="G207">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="H207">
+        <f t="shared" ref="H207:H213" si="198">I206</f>
+        <v>444</v>
+      </c>
+      <c r="I207">
+        <f t="shared" ref="I207:I213" si="199">H206</f>
+        <v>364</v>
+      </c>
+      <c r="J207">
+        <f t="shared" ref="J207:J213" si="200">K206</f>
+        <v>129</v>
+      </c>
+      <c r="K207">
+        <f t="shared" ref="K207:K213" si="201">J206</f>
+        <v>113</v>
+      </c>
+      <c r="L207">
+        <f t="shared" ref="L207:L213" si="202">M206</f>
+        <v>315</v>
+      </c>
+      <c r="M207">
+        <f t="shared" ref="M207:M213" si="203">L206</f>
+        <v>251</v>
+      </c>
+    </row>
+    <row r="208" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="B208" t="s">
-        <v>114</v>
+        <v>64</v>
       </c>
       <c r="C208">
         <v>2018</v>
       </c>
       <c r="D208" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="E208" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="F208">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G208">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="H208">
+        <v>342</v>
+      </c>
+      <c r="I208">
+        <v>199</v>
+      </c>
+      <c r="J208">
+        <v>190</v>
+      </c>
+      <c r="K208">
+        <v>-15</v>
+      </c>
+      <c r="L208">
+        <v>152</v>
+      </c>
+      <c r="M208">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="209" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="B209" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="C209">
         <v>2018</v>
       </c>
       <c r="D209" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="E209" t="s">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="F209">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="G209">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+      <c r="H209">
+        <f t="shared" ref="H209:H213" si="204">I208</f>
+        <v>199</v>
+      </c>
+      <c r="I209">
+        <f t="shared" ref="I209:I213" si="205">H208</f>
+        <v>342</v>
+      </c>
+      <c r="J209">
+        <f t="shared" ref="J209:J213" si="206">K208</f>
+        <v>-15</v>
+      </c>
+      <c r="K209">
+        <f t="shared" ref="K209:K213" si="207">J208</f>
+        <v>190</v>
+      </c>
+      <c r="L209">
+        <f t="shared" ref="L209:L213" si="208">M208</f>
+        <v>214</v>
+      </c>
+      <c r="M209">
+        <f t="shared" ref="M209:M213" si="209">L208</f>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="210" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="B210" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="C210">
         <v>2018</v>
       </c>
       <c r="D210" t="s">
-        <v>79</v>
+        <v>27</v>
       </c>
       <c r="E210" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="F210">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="G210">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="H210">
+        <v>297</v>
+      </c>
+      <c r="I210">
+        <v>407</v>
+      </c>
+      <c r="J210">
+        <v>176</v>
+      </c>
+      <c r="K210">
+        <v>161</v>
+      </c>
+      <c r="L210">
+        <v>121</v>
+      </c>
+      <c r="M210">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="211" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B211" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C211">
         <v>2018</v>
       </c>
       <c r="D211" t="s">
-        <v>79</v>
+        <v>27</v>
       </c>
       <c r="E211" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="F211">
+        <v>24</v>
+      </c>
+      <c r="G211">
         <v>27</v>
       </c>
-      <c r="G211">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H211">
+        <f t="shared" ref="H211:H213" si="210">I210</f>
+        <v>407</v>
+      </c>
+      <c r="I211">
+        <f t="shared" ref="I211:I213" si="211">H210</f>
+        <v>297</v>
+      </c>
+      <c r="J211">
+        <f t="shared" ref="J211:J213" si="212">K210</f>
+        <v>161</v>
+      </c>
+      <c r="K211">
+        <f t="shared" ref="K211:K213" si="213">J210</f>
+        <v>176</v>
+      </c>
+      <c r="L211">
+        <f t="shared" ref="L211:L213" si="214">M210</f>
+        <v>246</v>
+      </c>
+      <c r="M211">
+        <f t="shared" ref="M211:M213" si="215">L210</f>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="212" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="B212" t="s">
-        <v>86</v>
+        <v>26</v>
       </c>
       <c r="C212">
         <v>2018</v>
       </c>
       <c r="D212" t="s">
-        <v>27</v>
+        <v>136</v>
       </c>
       <c r="E212" t="s">
-        <v>175</v>
+        <v>13</v>
       </c>
       <c r="F212">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="G212">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="H212">
+        <v>482</v>
+      </c>
+      <c r="I212">
+        <v>443</v>
+      </c>
+      <c r="J212">
+        <v>135</v>
+      </c>
+      <c r="K212">
+        <v>148</v>
+      </c>
+      <c r="L212">
+        <v>347</v>
+      </c>
+      <c r="M212">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="213" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>175</v>
+        <v>13</v>
       </c>
       <c r="B213" t="s">
-        <v>207</v>
+        <v>14</v>
       </c>
       <c r="C213">
         <v>2018</v>
       </c>
       <c r="D213" t="s">
-        <v>27</v>
+        <v>136</v>
       </c>
       <c r="E213" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="F213">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="G213">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A214" t="s">
-        <v>45</v>
-      </c>
-      <c r="B214" t="s">
-        <v>26</v>
-      </c>
-      <c r="C214">
-        <v>2018</v>
-      </c>
-      <c r="D214" t="s">
-        <v>136</v>
-      </c>
-      <c r="E214" t="s">
-        <v>13</v>
-      </c>
-      <c r="F214">
         <v>44</v>
       </c>
-      <c r="G214">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A215" t="s">
-        <v>13</v>
-      </c>
-      <c r="B215" t="s">
-        <v>14</v>
-      </c>
-      <c r="C215">
-        <v>2018</v>
-      </c>
-      <c r="D215" t="s">
-        <v>136</v>
-      </c>
-      <c r="E215" t="s">
-        <v>45</v>
-      </c>
-      <c r="F215">
-        <v>16</v>
-      </c>
-      <c r="G215">
-        <v>44</v>
+      <c r="H213">
+        <f t="shared" ref="H213" si="216">I212</f>
+        <v>443</v>
+      </c>
+      <c r="I213">
+        <f t="shared" ref="I213" si="217">H212</f>
+        <v>482</v>
+      </c>
+      <c r="J213">
+        <f t="shared" ref="J213" si="218">K212</f>
+        <v>148</v>
+      </c>
+      <c r="K213">
+        <f t="shared" ref="K213" si="219">J212</f>
+        <v>135</v>
+      </c>
+      <c r="L213">
+        <f t="shared" ref="L213" si="220">M212</f>
+        <v>295</v>
+      </c>
+      <c r="M213">
+        <f t="shared" ref="M213" si="221">L212</f>
+        <v>347</v>
       </c>
     </row>
   </sheetData>

</xml_diff>